<commit_message>
Refatorado tratamento de datas para escrita de arquivos xlsx
</commit_message>
<xml_diff>
--- a/doc/RECORTE DIGITAL_BA-GO-DF - DISP 01-10-2025.xlsx
+++ b/doc/RECORTE DIGITAL_BA-GO-DF - DISP 01-10-2025.xlsx
@@ -33,7 +33,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -55,6 +55,21 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <color rgb="006100"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color rgb="006100"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color rgb="006100"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <color rgb="9C0006"/>
     </font>
     <font>
@@ -68,7 +83,7 @@
       <color rgb="9C0006"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none">
         <bgColor/>
@@ -88,6 +103,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0F243E"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor/>
       </patternFill>
     </fill>
@@ -129,7 +162,7 @@
   <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -138,6 +171,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +550,10 @@
         <v>BA</v>
       </c>
       <c r="C2" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D2" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E2" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-BA</v>
@@ -546,10 +582,10 @@
         <v>BA</v>
       </c>
       <c r="C3" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D3" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E3" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-BA</v>
@@ -578,10 +614,10 @@
         <v>BA</v>
       </c>
       <c r="C4" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D4" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E4" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - TJBA</v>
@@ -610,10 +646,10 @@
         <v>GO</v>
       </c>
       <c r="C5" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D5" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E5" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -642,10 +678,10 @@
         <v>GO</v>
       </c>
       <c r="C6" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D6" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E6" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -667,34 +703,34 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="str">
+      <c r="A7" s="8" t="str">
         <v>8588306372</v>
       </c>
-      <c r="B7" s="6" t="str">
+      <c r="B7" s="9" t="str">
         <v>GO</v>
       </c>
-      <c r="C7" s="7">
-        <v>45937.12273145833</v>
-      </c>
-      <c r="D7" s="7">
-        <v>45938.12273145833</v>
-      </c>
-      <c r="E7" s="6" t="str">
+      <c r="C7" s="10">
+        <v>45931</v>
+      </c>
+      <c r="D7" s="10">
+        <v>45932</v>
+      </c>
+      <c r="E7" s="9" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
       </c>
-      <c r="F7" s="6" t="str">
+      <c r="F7" s="9" t="str">
         <v>350004</v>
       </c>
-      <c r="G7" s="6" t="str">
+      <c r="G7" s="9" t="str">
         <v>1008384-60.2025.4.01.3502</v>
       </c>
-      <c r="H7" s="6" t="str">
+      <c r="H7" s="9" t="str">
         <v>Juizado Especial Cível e Criminal Adjunto à 1ª Vara Federal da SSJ de Anápolis-GO</v>
       </c>
-      <c r="I7" s="6" t="str">
+      <c r="I7" s="9" t="str">
         <v xml:space="preserve">Intimação  BR  PROCESSO: 1008384-60.2025.4.01.3502 - PROCEDIMENTO DO JUIZADO ESPECIAL CiVEL -  BR  || Subsecao Judiciaria de Anapolis-GO Juizado Especial Civel e Criminal Adjunto a 1ª Vara Federal da SSJ de Anapolis GO INTIMACAO VIA DIARIO ELETRONICO PROCESSO: 1008384-60.2025.4.01.3502 CLASSE: PROCEDIMENTO DO JUIZADO ESPECIAL CIVEL (436) POLO ATIVO: CRISTINA MARINHO DOS SANTOS REPRESENTANTES POLO ATIVO: FABIO CORREA RIBEIRO - MT6215/O POLO PASSIVO: INSTITUTO NACIONAL DO SEGURO SOCIAL - INSS Destinatarios: CRISTINA MARINHO DOS SANTOS FABIO CORREA RIBEIRO - (OAB: MT6215/O) FINALIDADE: Intimar a(s) parte(s) indicadas acerca do(a) ato ordinatorio / despacho / decisao / sentenca proferido(a) nos autos do processo em epigrafe. OBSERVACAO: Quando da resposta a este expediente, deve ser selecionada a intimacao a que ela se refere no campo  Marque os expedientes que pretende responder com esta peticao , sob pena de o sistema nao vincular a peticao de resposta a intimacao, com o consequente lancamento de decurso de prazo. Para maiores informacoes, favor consultar o Manual do PJe para Advogados e Procuradores em http: //portal.trf1.jus.br/portaltrf1/processual/processo-judicial-eletronico/pje/tutoriais. ANAPOLIS, 30 de setembro de 2025. (assinado digitalmente) Juizado Especial Civel e Criminal Adjunto a 1ª Vara Federal da SSJ de Anapolis-GO |||  BR  POLO ATIVO: CRISTINA MARINHO DOS SANTOS  BR  ADVOGADO: FABIO CORREA RIBEIRO - OAB: 6215/O/MT  BR  Acesso ao documento: https://pje1g.trf1.jus.br:443/pje/Processo/ConsultaDocumento/listView.seam?x=25093017395005900000059244536  BR  Identificador do documento: 420350004  BR </v>
       </c>
-      <c r="J7" s="6" t="str">
+      <c r="J7" s="9" t="str">
         <v xml:space="preserve">	</v>
       </c>
     </row>
@@ -706,10 +742,10 @@
         <v>GO</v>
       </c>
       <c r="C8" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D8" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E8" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -738,10 +774,10 @@
         <v>GO</v>
       </c>
       <c r="C9" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D9" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E9" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -770,10 +806,10 @@
         <v>GO</v>
       </c>
       <c r="C10" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D10" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E10" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -802,10 +838,10 @@
         <v>GO</v>
       </c>
       <c r="C11" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D11" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E11" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -834,10 +870,10 @@
         <v>GO</v>
       </c>
       <c r="C12" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D12" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E12" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -866,10 +902,10 @@
         <v>GO</v>
       </c>
       <c r="C13" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D13" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E13" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -898,10 +934,10 @@
         <v>GO</v>
       </c>
       <c r="C14" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D14" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E14" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -930,10 +966,10 @@
         <v>GO</v>
       </c>
       <c r="C15" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D15" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E15" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -962,10 +998,10 @@
         <v>GO</v>
       </c>
       <c r="C16" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D16" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E16" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -994,10 +1030,10 @@
         <v>GO</v>
       </c>
       <c r="C17" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D17" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E17" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-GO</v>
@@ -1026,10 +1062,10 @@
         <v>GO</v>
       </c>
       <c r="C18" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D18" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E18" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - TJGO</v>
@@ -1058,10 +1094,10 @@
         <v>GO</v>
       </c>
       <c r="C19" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D19" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E19" s="6" t="str">
         <v>Tribunal de Justiça Suplemento</v>
@@ -1087,10 +1123,10 @@
         <v>DJ</v>
       </c>
       <c r="C20" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D20" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E20" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - TJDFT</v>
@@ -1112,34 +1148,34 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="str">
+      <c r="A21" s="9" t="str">
         <v>8588600679</v>
       </c>
-      <c r="B21" s="6" t="str">
-        <v>DJ</v>
-      </c>
-      <c r="C21" s="7">
-        <v>45937.12273145833</v>
-      </c>
-      <c r="D21" s="7">
-        <v>45938.12273145833</v>
-      </c>
-      <c r="E21" s="6" t="str">
+      <c r="B21" s="9" t="str">
+        <v>DJ</v>
+      </c>
+      <c r="C21" s="10">
+        <v>45931</v>
+      </c>
+      <c r="D21" s="10">
+        <v>45932</v>
+      </c>
+      <c r="E21" s="9" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - TJDFT</v>
       </c>
-      <c r="F21" s="6" t="str">
+      <c r="F21" s="9" t="str">
         <v>1167</v>
       </c>
-      <c r="G21" s="6" t="str">
+      <c r="G21" s="9" t="str">
         <v>0719151-59.2021.8.07.0015</v>
       </c>
-      <c r="H21" s="6" t="str">
+      <c r="H21" s="9" t="str">
         <v>Vara de Ações Previdenciárias do DF</v>
       </c>
-      <c r="I21" s="6" t="str">
+      <c r="I21" s="9" t="str">
         <v xml:space="preserve">Intimação  BR  PROCESSO: 0719151-59.2021.8.07.0015 - CUMPRIMENTO DE SENTENcA CONTRA A FAZENDA PuBLICA -  BR  || Poder Judiciario da Uniao TRIBUNAL DE JUSTICA DO DISTRITO FEDERAL E DOS TERRITORIOS VAP Vara de Acoes Previdenciarias do DF Numero do processo: 0719151-59.2021.8.07.0015 Classe judicial: CUMPRIMENTO DE SENTENCA CONTRA A FAZENDA PUBLICA (12078) EXEQUENTE: MARIA EUGENIA LUCENA DOS SANTOS EXECUTADO: INSTITUTO NACIONAL DO SEGURO SOCIAL DESPACHO O historico de creditos ora juntado nao contempla o primeiro pagamento no valor revisado de R$ 1.968,94, que esta com data prevista para ser efetivamente realizado em 06/10/2025. Assim sendo, concedo a exequente derradeira oportunidade para juntar o historico de credito que contenha o pagamento da competencia 09/2025, efetivamente realizado. Int. Data e hora da assinatura digital. Vitor Feltrim Barbosa Juiz de Direito |||  BR  POLO ATIVO: MARIA EUGENIA LUCENA DOS SANTOS  BR  ADVOGADO: FABIO CORREA RIBEIRO - OAB: 035029/DF  BR  Acesso ao documento: https://pje.tjdft.jus.br/pje/Processo/ConsultaDocumento/listView.seam?x=25092918010486400000228496089  BR  Identificador do documento: 419201167  BR </v>
       </c>
-      <c r="J21" s="6" t="str">
+      <c r="J21" s="9" t="str">
         <v xml:space="preserve">	</v>
       </c>
     </row>
@@ -1151,10 +1187,10 @@
         <v>DJ</v>
       </c>
       <c r="C22" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D22" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E22" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - TRF1</v>
@@ -1183,10 +1219,10 @@
         <v>DJ</v>
       </c>
       <c r="C23" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D23" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E23" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - TRF1</v>
@@ -1215,10 +1251,10 @@
         <v>DJ</v>
       </c>
       <c r="C24" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D24" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E24" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - TRF1</v>
@@ -1247,10 +1283,10 @@
         <v>DJ</v>
       </c>
       <c r="C25" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D25" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E25" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - TRF1</v>
@@ -1279,10 +1315,10 @@
         <v>DJ</v>
       </c>
       <c r="C26" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D26" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E26" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-DF</v>
@@ -1311,10 +1347,10 @@
         <v>DJ</v>
       </c>
       <c r="C27" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D27" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E27" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-DF</v>
@@ -1343,10 +1379,10 @@
         <v>DJ</v>
       </c>
       <c r="C28" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D28" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E28" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-DF</v>
@@ -1375,10 +1411,10 @@
         <v>DJ</v>
       </c>
       <c r="C29" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D29" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E29" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-DF</v>
@@ -1407,10 +1443,10 @@
         <v>DJ</v>
       </c>
       <c r="C30" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D30" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E30" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-DF</v>
@@ -1439,10 +1475,10 @@
         <v>DJ</v>
       </c>
       <c r="C31" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D31" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E31" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-DF</v>
@@ -1471,10 +1507,10 @@
         <v>DJ</v>
       </c>
       <c r="C32" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D32" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E32" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-DF</v>
@@ -1503,10 +1539,10 @@
         <v>DJ</v>
       </c>
       <c r="C33" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D33" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E33" s="6" t="str">
         <v>DJEN - Diário de Justiça Eletrônico Nacional - JFED-DF</v>
@@ -1535,10 +1571,10 @@
         <v>DJ</v>
       </c>
       <c r="C34" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D34" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E34" s="6" t="str">
         <v>Tribunal Superior do Trabalho DJEN - Diário de Justiça Eletrônico Nacional - TST</v>
@@ -1567,10 +1603,10 @@
         <v>DJ</v>
       </c>
       <c r="C35" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D35" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E35" s="6" t="str">
         <v>Tribunal Superior do Trabalho DJEN - Diário de Justiça Eletrônico Nacional - TST</v>
@@ -1599,10 +1635,10 @@
         <v>DJ</v>
       </c>
       <c r="C36" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D36" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E36" s="6" t="str">
         <v>Tribunal Superior do Trabalho DJEN - Diário de Justiça Eletrônico Nacional - TST</v>
@@ -1631,10 +1667,10 @@
         <v>DJ</v>
       </c>
       <c r="C37" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D37" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E37" s="6" t="str">
         <v>Tribunal Superior do Trabalho DJEN - Diário de Justiça Eletrônico Nacional - TST</v>
@@ -1663,10 +1699,10 @@
         <v>DJ</v>
       </c>
       <c r="C38" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D38" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E38" s="6" t="str">
         <v>Tribunal Superior do Trabalho DJEN - Diário de Justiça Eletrônico Nacional - TST</v>
@@ -1695,10 +1731,10 @@
         <v>DJ</v>
       </c>
       <c r="C39" s="7">
-        <v>45937.12273145833</v>
+        <v>45931</v>
       </c>
       <c r="D39" s="7">
-        <v>45938.12273145833</v>
+        <v>45932</v>
       </c>
       <c r="E39" s="6" t="str">
         <v>Tribunal Superior do Trabalho DJEN - Diário de Justiça Eletrônico Nacional - TST</v>

</xml_diff>